<commit_message>
updated Apr 2023 data
</commit_message>
<xml_diff>
--- a/data/Early Career Fac Apr2023.xlsx
+++ b/data/Early Career Fac Apr2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/early_career_faculty/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA1F287-E28B-B545-8291-20A21E9BC3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED687070-D863-7440-910B-3172CC4B2C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="16140" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="16120" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="281">
   <si>
     <t>Name</t>
   </si>
@@ -809,9 +809,6 @@
     <t>Carpenter, Eileen</t>
   </si>
   <si>
-    <t>INSTRUCTOR</t>
-  </si>
-  <si>
     <t>Berinstein, Jeff</t>
   </si>
   <si>
@@ -827,33 +824,6 @@
     <t>Mazumder, Nikilesh</t>
   </si>
   <si>
-    <t>I should find out about score in October and then funding starting in April if funded.</t>
-  </si>
-  <si>
-    <t>K resubmission July 2022, Score Oct, Fund April 2023</t>
-  </si>
-  <si>
-    <t>Resubmit R01 Oct or Feb, Resub R with Wisc in Dec, K-related R sub in June, score Oct22</t>
-  </si>
-  <si>
-    <t>Submit R01 Oct22 or Feb23</t>
-  </si>
-  <si>
-    <t>CCF CDA submitted in July 2022 -&gt; hear back in November 2022</t>
-  </si>
-  <si>
-    <t>Rebuttal letter for this K23 cycle due August 15</t>
-  </si>
-  <si>
-    <t>Submission K23 October 2022 -&gt; hear back in March 2023 -&gt; Resubmit if necessary in July 2023</t>
-  </si>
-  <si>
-    <t>AGA RSA November 2022 -&gt; hear back in April 2023</t>
-  </si>
-  <si>
-    <t>Rebuttal letter for this K23 cycle due August 15, CCF CDA score  in Nov22, Submission K23 October 2022 -&gt; hear back in March 2023 -&gt; Resubmit if necessary in July 2023, AGA RSA November 2022 -&gt; hear back in April 2023</t>
-  </si>
-  <si>
     <t>New K08 subm 6/22, score Nov 22, start funding Apr 23</t>
   </si>
   <si>
@@ -864,6 +834,36 @@
   </si>
   <si>
     <t>R01 submit June 2023</t>
+  </si>
+  <si>
+    <t>first R01 submission fall 2024</t>
+  </si>
+  <si>
+    <t>submitting K08 in June</t>
+  </si>
+  <si>
+    <t>submit R03 in June, R01 In fall 2024</t>
+  </si>
+  <si>
+    <t>R03 funded, R01 submit June 2024</t>
+  </si>
+  <si>
+    <t>Submit R01s Oct 2023, Feb 2024</t>
+  </si>
+  <si>
+    <t>Submit K fall 2023</t>
+  </si>
+  <si>
+    <t>K23 resub July 2023m IIR in Dec 23, has 8/8ths VA</t>
+  </si>
+  <si>
+    <t>R01 AA030748, sole PI, R01 AA030969 JIT received, R01 AA030470  resub April23</t>
+  </si>
+  <si>
+    <t>received JIT</t>
+  </si>
+  <si>
+    <t>Newman, Kira</t>
   </si>
 </sst>
 </file>
@@ -922,7 +922,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,6 +938,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,7 +1027,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1085,6 +1091,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3565,10 +3574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25382A1C-1D0F-5146-80FF-DF6BAF2EBCFA}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3597,12 +3606,12 @@
         <v>254</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>16</v>
@@ -3619,7 +3628,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>16</v>
@@ -3651,7 +3660,7 @@
         <v>43281</v>
       </c>
       <c r="F4" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -3671,7 +3680,7 @@
         <v>44012</v>
       </c>
       <c r="F5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -3696,7 +3705,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>255</v>
@@ -3707,16 +3716,14 @@
       <c r="E7" s="17">
         <v>45473</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>269</v>
-      </c>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>259</v>
@@ -3728,7 +3735,7 @@
         <v>45107</v>
       </c>
       <c r="F8" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3736,7 +3743,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>255</v>
@@ -3748,7 +3755,7 @@
         <v>44012</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -3756,7 +3763,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>258</v>
@@ -3773,7 +3780,7 @@
         <v>261</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>255</v>
@@ -3790,7 +3797,7 @@
         <v>261</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>259</v>
@@ -3807,10 +3814,10 @@
         <v>261</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D13" s="17">
         <v>44563</v>
@@ -3818,16 +3825,14 @@
       <c r="E13" s="17">
         <v>46386</v>
       </c>
-      <c r="F13" s="25" t="s">
-        <v>272</v>
-      </c>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>255</v>
@@ -3838,16 +3843,14 @@
       <c r="E14" s="17">
         <v>44742</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>273</v>
-      </c>
+      <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>257</v>
@@ -3858,16 +3861,14 @@
       <c r="E15" s="17">
         <v>46568</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>274</v>
-      </c>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>260</v>
@@ -3878,16 +3879,14 @@
       <c r="E16" s="17">
         <v>44742</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>275</v>
-      </c>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>255</v>
@@ -3904,7 +3903,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>258</v>
@@ -3941,7 +3940,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D20" s="17">
         <v>43891</v>
@@ -3950,7 +3949,7 @@
         <v>44620</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -3958,7 +3957,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>255</v>
@@ -3973,88 +3972,89 @@
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D22" s="17">
-        <v>42917</v>
+        <v>45017</v>
       </c>
       <c r="E22" s="17">
-        <v>44012</v>
+        <v>46843</v>
       </c>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="27" t="s">
         <v>81</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="17">
+        <v>42917</v>
+      </c>
+      <c r="E23" s="17">
+        <v>44012</v>
+      </c>
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D24" s="17">
         <v>43647</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E24" s="17">
         <v>45107</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="D24" s="17">
-        <v>42186</v>
-      </c>
-      <c r="E24" s="17">
-        <v>43281</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="27" t="s">
         <v>175</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D25" s="17">
-        <v>43647</v>
+        <v>42186</v>
       </c>
       <c r="E25" s="17">
-        <v>45412</v>
+        <v>43281</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="15" t="s">
-        <v>177</v>
+      <c r="A26" s="27" t="s">
+        <v>175</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D26" s="17">
-        <v>42186</v>
+        <v>43647</v>
       </c>
       <c r="E26" s="17">
-        <v>42916</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -4065,13 +4065,13 @@
         <v>16</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D27" s="17">
-        <v>42795</v>
+        <v>42186</v>
       </c>
       <c r="E27" s="17">
-        <v>43889</v>
+        <v>42916</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -4082,33 +4082,33 @@
         <v>16</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D28" s="17">
-        <v>44274</v>
+        <v>42795</v>
       </c>
       <c r="E28" s="17">
-        <v>45350</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>270</v>
+        <v>43889</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="15" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D29" s="17">
-        <v>42186</v>
+        <v>44274</v>
       </c>
       <c r="E29" s="17">
-        <v>43281</v>
+        <v>45350</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -4119,10 +4119,10 @@
         <v>16</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D30" s="17">
-        <v>42552</v>
+        <v>42186</v>
       </c>
       <c r="E30" s="17">
         <v>43281</v>
@@ -4136,33 +4136,33 @@
         <v>16</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D31" s="17">
-        <v>43282</v>
+        <v>42552</v>
       </c>
       <c r="E31" s="17">
-        <v>45107</v>
+        <v>43281</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="15" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D32" s="17">
-        <v>42125</v>
-      </c>
-      <c r="E32" s="19">
-        <v>43281</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>271</v>
+        <v>43282</v>
+      </c>
+      <c r="E32" s="17">
+        <v>45107</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -4173,33 +4173,33 @@
         <v>16</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D33" s="17">
-        <v>43692</v>
-      </c>
-      <c r="E33" s="17">
-        <v>45443</v>
+        <v>42125</v>
+      </c>
+      <c r="E33" s="19">
+        <v>43281</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D34" s="17">
-        <v>42552</v>
+        <v>43692</v>
       </c>
       <c r="E34" s="17">
-        <v>43646</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>277</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -4210,98 +4210,182 @@
         <v>13</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D35" s="17">
-        <v>43525</v>
+        <v>42552</v>
       </c>
       <c r="E35" s="17">
-        <v>44255</v>
+        <v>43646</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D36" s="17">
-        <v>43678</v>
+        <v>43525</v>
       </c>
       <c r="E36" s="17">
-        <v>44773</v>
-      </c>
+        <v>44255</v>
+      </c>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="15" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D37" s="17">
-        <v>43709</v>
+        <v>45108</v>
       </c>
       <c r="E37" s="17">
-        <v>44804</v>
+        <v>46568</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38" s="17">
+        <v>43678</v>
+      </c>
+      <c r="E38" s="17">
+        <v>44773</v>
+      </c>
+      <c r="F38" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B39" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C39" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D39" s="17">
+        <v>43709</v>
+      </c>
+      <c r="E39" s="17">
+        <v>44804</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D40" s="17">
         <v>44378</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E40" s="17">
         <v>46203</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B39" s="22" t="s">
+      <c r="F40" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B41" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C41" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D41" s="24">
         <v>44743</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E41" s="24">
         <v>45473</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B40" s="22" t="s">
+      <c r="F41" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B42" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C42" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D42" s="24">
         <v>44743</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E42" s="24">
         <v>45838</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="D43" s="24">
+        <v>45108</v>
+      </c>
+      <c r="E43" s="24">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="D44" s="24">
+        <v>45108</v>
+      </c>
+      <c r="E44" s="24">
+        <v>46203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updted for April 2024
</commit_message>
<xml_diff>
--- a/data/Early Career Fac Apr2023.xlsx
+++ b/data/Early Career Fac Apr2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/early_career_faculty/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED687070-D863-7440-910B-3172CC4B2C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F9D93-7136-2F4E-9538-FA476F82FFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="16120" windowWidth="21600" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="279">
   <si>
     <t>Name</t>
   </si>
@@ -824,30 +824,12 @@
     <t>Mazumder, Nikilesh</t>
   </si>
   <si>
-    <t>New K08 subm 6/22, score Nov 22, start funding Apr 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K23 response July 23 </t>
-  </si>
-  <si>
-    <t>R03 results June 2023</t>
-  </si>
-  <si>
-    <t>R01 submit June 2023</t>
-  </si>
-  <si>
     <t>first R01 submission fall 2024</t>
   </si>
   <si>
-    <t>submitting K08 in June</t>
-  </si>
-  <si>
     <t>submit R03 in June, R01 In fall 2024</t>
   </si>
   <si>
-    <t>R03 funded, R01 submit June 2024</t>
-  </si>
-  <si>
     <t>Submit R01s Oct 2023, Feb 2024</t>
   </si>
   <si>
@@ -857,13 +839,25 @@
     <t>K23 resub July 2023m IIR in Dec 23, has 8/8ths VA</t>
   </si>
   <si>
-    <t>R01 AA030748, sole PI, R01 AA030969 JIT received, R01 AA030470  resub April23</t>
-  </si>
-  <si>
-    <t>received JIT</t>
-  </si>
-  <si>
     <t>Newman, Kira</t>
+  </si>
+  <si>
+    <t>K23 close July 23 - resub Nov 23</t>
+  </si>
+  <si>
+    <t>R01 submit Oct 2023</t>
+  </si>
+  <si>
+    <t>R03 NF</t>
+  </si>
+  <si>
+    <t>R01 AA030748, sole PI, R01 AA030969 JIT received, R01 AA030470  funded</t>
+  </si>
+  <si>
+    <t>K23 funded 2023</t>
+  </si>
+  <si>
+    <t>R03 funded, R01 funded 2024</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1092,6 +1086,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3577,7 +3574,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3659,12 +3656,12 @@
       <c r="E4" s="17">
         <v>43281</v>
       </c>
-      <c r="F4" t="s">
-        <v>269</v>
+      <c r="F4" s="20" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -3679,8 +3676,8 @@
       <c r="E5" s="17">
         <v>44012</v>
       </c>
-      <c r="F5" t="s">
-        <v>270</v>
+      <c r="F5" s="20" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -3734,8 +3731,8 @@
       <c r="E8" s="17">
         <v>45107</v>
       </c>
-      <c r="F8" t="s">
-        <v>268</v>
+      <c r="F8" s="20" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3755,7 +3752,7 @@
         <v>44012</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -3828,7 +3825,7 @@
       <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -3846,7 +3843,7 @@
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>54</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -3949,7 +3946,7 @@
         <v>44620</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -4108,7 +4105,7 @@
         <v>45350</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -4145,7 +4142,7 @@
         <v>43281</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -4182,7 +4179,7 @@
         <v>43281</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -4218,9 +4215,7 @@
       <c r="E35" s="17">
         <v>43646</v>
       </c>
-      <c r="F35" s="20" t="s">
-        <v>267</v>
-      </c>
+      <c r="F35" s="20"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="15" t="s">
@@ -4257,11 +4252,11 @@
         <v>46568</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="27" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -4275,9 +4270,6 @@
       </c>
       <c r="E38" s="17">
         <v>44773</v>
-      </c>
-      <c r="F38" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -4314,7 +4306,7 @@
         <v>46203</v>
       </c>
       <c r="F40" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -4334,7 +4326,7 @@
         <v>45473</v>
       </c>
       <c r="F41" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
@@ -4356,7 +4348,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="22" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>13</v>
@@ -4373,7 +4365,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="22" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>13</v>

</xml_diff>